<commit_message>
Updateing the spreasheets for 180 users and 7 votations
</commit_message>
<xml_diff>
--- a/data/feedback.xlsx
+++ b/data/feedback.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t>2</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Due attendance</t>
   </si>
   <si>
-    <t>100</t>
+    <t>180</t>
   </si>
   <si>
     <t>1</t>
@@ -64,19 +64,19 @@
     <t xml:space="preserve">Yes </t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>46.4%</t>
+    <t>81</t>
+  </si>
+  <si>
+    <t>45.0%</t>
   </si>
   <si>
     <t xml:space="preserve"> No</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>53.6%</t>
+    <t>99</t>
+  </si>
+  <si>
+    <t>55.0%</t>
   </si>
   <si>
     <t>Participants</t>
@@ -85,12 +85,6 @@
     <t>Submitted</t>
   </si>
   <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>84.0%</t>
-  </si>
-  <si>
     <t>Correct Answer</t>
   </si>
   <si>
@@ -112,25 +106,31 @@
     <t>4</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>26.1%</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>28.3%</t>
+    <t>87</t>
+  </si>
+  <si>
+    <t>24.2%</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>25.8%</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>16.9%</t>
-  </si>
-  <si>
-    <t>18.3%</t>
+    <t>94</t>
+  </si>
+  <si>
+    <t>17.4%</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>15.9%</t>
   </si>
   <si>
     <t>7</t>
@@ -139,52 +139,43 @@
     <t xml:space="preserve">True </t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>13.0%</t>
+    <t>11.9%</t>
   </si>
   <si>
     <t xml:space="preserve"> False</t>
   </si>
   <si>
+    <t>13.1%</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
     <t xml:space="preserve">Right </t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>10.3%</t>
+    <t>10.4%</t>
   </si>
   <si>
     <t xml:space="preserve"> Wrong</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>9.2%</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>93.0%</t>
+    <t>9.6%</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>8.1%</t>
+    <t>105</t>
+  </si>
+  <si>
+    <t>9.7%</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>6.9%</t>
   </si>
 </sst>
 </file>
@@ -682,15 +673,15 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -698,7 +689,7 @@
     </row>
     <row r="14" spans="1:4" ht="18" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -710,20 +701,20 @@
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="18" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -731,7 +722,7 @@
     <row r="17" spans="1:4" ht="18" customHeight="1"/>
     <row r="18" spans="1:4" ht="18" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -757,10 +748,10 @@
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1">
@@ -771,10 +762,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1">
@@ -801,7 +792,7 @@
     </row>
     <row r="24" spans="1:4" ht="18" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -809,7 +800,7 @@
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -821,20 +812,20 @@
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="18" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -842,7 +833,7 @@
     <row r="28" spans="1:4" ht="18" customHeight="1"/>
     <row r="29" spans="1:4" ht="18" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
@@ -868,10 +859,10 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18" customHeight="1">
@@ -882,7 +873,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>38</v>
@@ -912,7 +903,7 @@
     </row>
     <row r="35" spans="1:4" ht="18" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -920,7 +911,7 @@
     </row>
     <row r="36" spans="1:4" ht="18" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -932,20 +923,20 @@
     </row>
     <row r="37" spans="1:4" ht="18" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="18" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -979,10 +970,10 @@
         <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18" customHeight="1">
@@ -990,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18" customHeight="1">
@@ -1023,7 +1014,7 @@
     </row>
     <row r="46" spans="1:4" ht="18" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1031,7 +1022,7 @@
     </row>
     <row r="47" spans="1:4" ht="18" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
@@ -1043,20 +1034,20 @@
     </row>
     <row r="48" spans="1:4" ht="18" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="18" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1090,10 +1081,10 @@
         <v>45</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" customHeight="1">
@@ -1101,13 +1092,13 @@
         <v>0</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" customHeight="1">
@@ -1126,15 +1117,15 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1142,7 +1133,7 @@
     </row>
     <row r="58" spans="1:4" ht="18" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
@@ -1154,20 +1145,20 @@
     </row>
     <row r="59" spans="1:4" ht="18" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" ht="18" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1175,7 +1166,7 @@
     <row r="61" spans="1:4" ht="18" customHeight="1"/>
     <row r="62" spans="1:4" ht="18" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>13</v>
@@ -1201,10 +1192,10 @@
         <v>15</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" customHeight="1">
@@ -1215,10 +1206,10 @@
         <v>18</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1">
@@ -1245,7 +1236,7 @@
     </row>
     <row r="68" spans="1:4" ht="18" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1253,7 +1244,7 @@
     </row>
     <row r="69" spans="1:4" ht="18" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
@@ -1265,20 +1256,20 @@
     </row>
     <row r="70" spans="1:4" ht="18" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="18" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>

</xml_diff>